<commit_message>
new Classes and new tests
</commit_message>
<xml_diff>
--- a/docs/Cases.xlsx
+++ b/docs/Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andrey\qa-diplom\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF87CDD-215F-43C0-BFB6-480B68CB60D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E3E19-6AC9-44FA-BCCF-771F6976B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Набор тест кейсов по LogIn и Lo" sheetId="1" r:id="rId1"/>
@@ -722,28 +722,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -751,14 +734,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -769,11 +755,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -781,22 +764,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1120,23 +1120,23 @@
   </sheetPr>
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" customWidth="1"/>
-    <col min="7" max="7" width="49.109375" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="49.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1145,7 +1145,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1158,699 +1158,699 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="11" t="s">
+    <row r="3" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="11" t="s">
+    <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="15"/>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="15"/>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="32"/>
+      <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="11" t="s">
+    <row r="8" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11" t="s">
+    <row r="9" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="32"/>
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="11" t="s">
+    <row r="13" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="11" t="s">
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="11" t="s">
+      <c r="E17" s="32"/>
+      <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="25"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="11" t="s">
+      <c r="E23" s="32"/>
+      <c r="F23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="11" t="s">
+    <row r="24" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+    <row r="25" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-    </row>
-    <row r="29" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="25"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="11" t="s">
+      <c r="E29" s="32"/>
+      <c r="F29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="11" t="s">
+    <row r="30" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="25"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="11" t="s">
+      <c r="E35" s="32"/>
+      <c r="F35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="11" t="s">
+    <row r="36" spans="1:7" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="24"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="24"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="24"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="24"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="25"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="11" t="s">
+      <c r="E41" s="32"/>
+      <c r="F41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="11" t="s">
+    <row r="42" spans="1:7" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="24"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="11" t="s">
+    <row r="43" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="24"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G43" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="24"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="24"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="47" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="25"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="11" t="s">
+      <c r="E47" s="32"/>
+      <c r="F47" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="G47" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="11" t="s">
+    <row r="48" spans="1:7" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="24"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="11" t="s">
+    <row r="49" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="24"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="24"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="24"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="53" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="25"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="F53" s="11" t="s">
+      <c r="E53" s="32"/>
+      <c r="F53" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G53" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="11" t="s">
+    <row r="54" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="24"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G54" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+    <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="24"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="24"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="24"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-    </row>
-    <row r="59" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="34" t="s">
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="25"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="12" t="s">
         <v>160</v>
       </c>
       <c r="B59" s="18" t="s">
@@ -1859,71 +1859,71 @@
       <c r="C59" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="20"/>
-      <c r="F59" s="11" t="s">
+      <c r="E59" s="28"/>
+      <c r="F59" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="11" t="s">
+    <row r="60" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="24"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="11" t="s">
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="24"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="G61" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="17" t="s">
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="24"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="G62" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="17" t="s">
+    <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="25"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="G63" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
+    <row r="64" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="12" t="s">
         <v>161</v>
       </c>
       <c r="B64" s="18" t="s">
@@ -1932,67 +1932,67 @@
       <c r="C64" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="20"/>
-      <c r="F64" s="11" t="s">
+      <c r="E64" s="28"/>
+      <c r="F64" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G64" s="11" t="s">
+      <c r="G64" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="11" t="s">
+    <row r="65" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="24"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="11" t="s">
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="24"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="17" t="s">
+    <row r="67" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="24"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="G67" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-    </row>
-    <row r="69" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
+    <row r="68" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="25"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+    </row>
+    <row r="69" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="12" t="s">
         <v>162</v>
       </c>
       <c r="B69" s="18" t="s">
@@ -2001,71 +2001,71 @@
       <c r="C69" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="20"/>
-      <c r="F69" s="11" t="s">
+      <c r="E69" s="28"/>
+      <c r="F69" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="G69" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="30"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="11" t="s">
+    <row r="70" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="24"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G70" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="11" t="s">
+    <row r="71" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="24"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G71" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="17" t="s">
+    <row r="72" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="24"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G72" s="17" t="s">
+      <c r="G72" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="17" t="s">
+    <row r="73" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="25"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G73" s="17" t="s">
+      <c r="G73" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="34" t="s">
+    <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="12" t="s">
         <v>163</v>
       </c>
       <c r="B74" s="18" t="s">
@@ -2074,69 +2074,69 @@
       <c r="C74" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D74" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="21" t="s">
+      <c r="E74" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G74" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="11" t="s">
+    <row r="75" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="24"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="G75" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="17" t="s">
+    <row r="76" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="24"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="G76" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="17" t="s">
+    <row r="77" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="24"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G77" s="17" t="s">
+      <c r="G77" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-    </row>
-    <row r="79" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="34" t="s">
+    <row r="78" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="25"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="27"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+    </row>
+    <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="12" t="s">
         <v>164</v>
       </c>
       <c r="B79" s="18" t="s">
@@ -2145,905 +2145,795 @@
       <c r="C79" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="21" t="s">
+      <c r="E79" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="F79" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="G79" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="11" t="s">
+    <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="24"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G80" s="11" t="s">
+      <c r="G80" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="17" t="s">
+    <row r="81" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="24"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G81" s="17" t="s">
+      <c r="G81" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="17" t="s">
+    <row r="82" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="24"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G82" s="17" t="s">
+      <c r="G82" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="17" t="s">
+    <row r="83" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="25"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G83" s="17" t="s">
+      <c r="G83" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="34" t="s">
+    <row r="84" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="21" t="s">
+      <c r="B84" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C84" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="D84" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="21" t="s">
+      <c r="E84" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F84" s="11" t="s">
+      <c r="F84" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G84" s="11" t="s">
+      <c r="G84" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="11" t="s">
+    <row r="85" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="24"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="G85" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="17" t="s">
+    <row r="86" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="24"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G86" s="17" t="s">
+      <c r="G86" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="17" t="s">
+    <row r="87" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="24"/>
+      <c r="B87" s="26"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G87" s="17" t="s">
+      <c r="G87" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="17" t="s">
+    <row r="88" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="25"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G88" s="17" t="s">
+      <c r="G88" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="34" t="s">
+    <row r="89" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="15" t="s">
         <v>97</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="21" t="s">
+      <c r="E89" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="F89" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G89" s="11" t="s">
+      <c r="G89" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="11" t="s">
+    <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="24"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G90" s="11" t="s">
+      <c r="G90" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="30"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="17" t="s">
+    <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="24"/>
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G91" s="17" t="s">
+      <c r="G91" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="17" t="s">
+    <row r="92" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="24"/>
+      <c r="B92" s="26"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G92" s="17" t="s">
+      <c r="G92" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="31"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="17" t="s">
+    <row r="93" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="25"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G93" s="17" t="s">
+      <c r="G93" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="34" t="s">
+    <row r="94" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B94" s="21" t="s">
+      <c r="B94" s="15" t="s">
         <v>103</v>
       </c>
       <c r="C94" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D94" s="19" t="s">
+      <c r="D94" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="21" t="s">
+      <c r="E94" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F94" s="11" t="s">
+      <c r="F94" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G94" s="11" t="s">
+      <c r="G94" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="17" t="s">
+    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="24"/>
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G95" s="17" t="s">
+      <c r="G95" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="17" t="s">
+    <row r="96" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="24"/>
+      <c r="B96" s="26"/>
+      <c r="C96" s="26"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G96" s="17" t="s">
+      <c r="G96" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="17" t="s">
+    <row r="97" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="24"/>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G97" s="17" t="s">
+      <c r="G97" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
-    </row>
-    <row r="99" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="34" t="s">
+    <row r="98" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="25"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+    </row>
+    <row r="99" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="15" t="s">
         <v>110</v>
       </c>
       <c r="C99" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D99" s="19" t="s">
+      <c r="D99" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="21" t="s">
+      <c r="E99" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="F99" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G99" s="11" t="s">
+      <c r="G99" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="17" t="s">
+    <row r="100" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="24"/>
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G100" s="17" t="s">
+      <c r="G100" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="17" t="s">
+    <row r="101" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="24"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="G101" s="17" t="s">
+      <c r="G101" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="17" t="s">
+    <row r="102" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="24"/>
+      <c r="B102" s="26"/>
+      <c r="C102" s="26"/>
+      <c r="D102" s="26"/>
+      <c r="E102" s="26"/>
+      <c r="F102" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G102" s="17" t="s">
+      <c r="G102" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="31"/>
-      <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="13"/>
-      <c r="E103" s="13"/>
-      <c r="F103" s="17"/>
-      <c r="G103" s="17"/>
-    </row>
-    <row r="104" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="34" t="s">
+    <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="25"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+    </row>
+    <row r="104" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B104" s="21" t="s">
+      <c r="B104" s="15" t="s">
         <v>117</v>
       </c>
       <c r="C104" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D104" s="19" t="s">
+      <c r="D104" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="21" t="s">
+      <c r="E104" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="F104" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G104" s="11" t="s">
+      <c r="G104" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="30"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="17" t="s">
+    <row r="105" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="24"/>
+      <c r="B105" s="26"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="26"/>
+      <c r="F105" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G105" s="17" t="s">
+      <c r="G105" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="17" t="s">
+    <row r="106" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="24"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G106" s="17" t="s">
+      <c r="G106" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="30"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="17" t="s">
+    <row r="107" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="24"/>
+      <c r="B107" s="26"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G107" s="17" t="s">
+      <c r="G107" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="31"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="13"/>
-      <c r="F108" s="17"/>
-      <c r="G108" s="17"/>
-    </row>
-    <row r="109" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="34" t="s">
+    <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="25"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+    </row>
+    <row r="109" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="15" t="s">
         <v>128</v>
       </c>
       <c r="C109" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D109" s="19" t="s">
+      <c r="D109" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E109" s="21" t="s">
+      <c r="E109" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="F109" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="G109" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="30"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="17" t="s">
+    <row r="110" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="24"/>
+      <c r="B110" s="26"/>
+      <c r="C110" s="26"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G110" s="17" t="s">
+      <c r="G110" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="17" t="s">
+    <row r="111" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="24"/>
+      <c r="B111" s="26"/>
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="G111" s="17" t="s">
+      <c r="G111" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="17" t="s">
+    <row r="112" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="24"/>
+      <c r="B112" s="26"/>
+      <c r="C112" s="26"/>
+      <c r="D112" s="26"/>
+      <c r="E112" s="26"/>
+      <c r="F112" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G112" s="17" t="s">
+      <c r="G112" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="31"/>
-      <c r="B113" s="13"/>
-      <c r="C113" s="13"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="17"/>
-      <c r="G113" s="17"/>
-    </row>
-    <row r="114" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="34" t="s">
+    <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="25"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
+    </row>
+    <row r="114" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B114" s="21" t="s">
+      <c r="B114" s="15" t="s">
         <v>131</v>
       </c>
       <c r="C114" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D114" s="19" t="s">
+      <c r="D114" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E114" s="21" t="s">
+      <c r="E114" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F114" s="11" t="s">
+      <c r="F114" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G114" s="11" t="s">
+      <c r="G114" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="17" t="s">
+    <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="24"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G115" s="17" t="s">
+      <c r="G115" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="30"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="17" t="s">
+    <row r="116" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="24"/>
+      <c r="B116" s="26"/>
+      <c r="C116" s="26"/>
+      <c r="D116" s="26"/>
+      <c r="E116" s="26"/>
+      <c r="F116" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G116" s="17" t="s">
+      <c r="G116" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="17" t="s">
+    <row r="117" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="24"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="26"/>
+      <c r="F117" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G117" s="17" t="s">
+      <c r="G117" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
-      <c r="B118" s="13"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="13"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="17"/>
-      <c r="G118" s="17"/>
-    </row>
-    <row r="119" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="34" t="s">
+    <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="25"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="27"/>
+      <c r="D118" s="27"/>
+      <c r="E118" s="27"/>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
+    </row>
+    <row r="119" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B119" s="21" t="s">
+      <c r="B119" s="15" t="s">
         <v>137</v>
       </c>
       <c r="C119" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D119" s="19" t="s">
+      <c r="D119" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="21" t="s">
+      <c r="E119" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F119" s="11" t="s">
+      <c r="F119" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G119" s="11" t="s">
+      <c r="G119" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
-      <c r="B120" s="22"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="24"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="17" t="s">
+    <row r="120" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="13"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G120" s="17" t="s">
+      <c r="G120" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="32"/>
-      <c r="B121" s="22"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="24"/>
-      <c r="E121" s="22"/>
-      <c r="F121" s="17" t="s">
+    <row r="121" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="13"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G121" s="17" t="s">
+      <c r="G121" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="32"/>
-      <c r="B122" s="22"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="24"/>
-      <c r="E122" s="22"/>
-      <c r="F122" s="17" t="s">
+    <row r="122" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="13"/>
+      <c r="B122" s="16"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="22"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="G122" s="17" t="s">
+      <c r="G122" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="33"/>
-      <c r="B123" s="23"/>
-      <c r="C123" s="27"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="23"/>
-      <c r="F123" s="17"/>
-      <c r="G123" s="17"/>
-    </row>
-    <row r="124" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="34" t="s">
+    <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="14"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="20"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+    </row>
+    <row r="124" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="B124" s="21" t="s">
+      <c r="B124" s="15" t="s">
         <v>143</v>
       </c>
       <c r="C124" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D124" s="19" t="s">
+      <c r="D124" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E124" s="21" t="s">
+      <c r="E124" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F124" s="11" t="s">
+      <c r="F124" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G124" s="11" t="s">
+      <c r="G124" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="32"/>
-      <c r="B125" s="22"/>
-      <c r="C125" s="26"/>
-      <c r="D125" s="24"/>
-      <c r="E125" s="22"/>
-      <c r="F125" s="17" t="s">
+    <row r="125" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="13"/>
+      <c r="B125" s="16"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="22"/>
+      <c r="E125" s="16"/>
+      <c r="F125" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G125" s="17" t="s">
+      <c r="G125" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="32"/>
-      <c r="B126" s="22"/>
-      <c r="C126" s="26"/>
-      <c r="D126" s="24"/>
-      <c r="E126" s="22"/>
-      <c r="F126" s="17" t="s">
+    <row r="126" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="13"/>
+      <c r="B126" s="16"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="22"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G126" s="17" t="s">
+      <c r="G126" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="32"/>
-      <c r="B127" s="22"/>
-      <c r="C127" s="26"/>
-      <c r="D127" s="24"/>
-      <c r="E127" s="22"/>
-      <c r="F127" s="17" t="s">
+    <row r="127" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="13"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="22"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="G127" s="17" t="s">
+      <c r="G127" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="33"/>
-      <c r="B128" s="23"/>
-      <c r="C128" s="27"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="23"/>
-      <c r="F128" s="17"/>
-      <c r="G128" s="17"/>
-    </row>
-    <row r="129" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="34" t="s">
+    <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="14"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="10"/>
+      <c r="G128" s="10"/>
+    </row>
+    <row r="129" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B129" s="21" t="s">
+      <c r="B129" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C129" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D129" s="19" t="s">
+      <c r="D129" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E129" s="21" t="s">
+      <c r="E129" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F129" s="11" t="s">
+      <c r="F129" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G129" s="11" t="s">
+      <c r="G129" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="32"/>
-      <c r="B130" s="22"/>
-      <c r="C130" s="26"/>
-      <c r="D130" s="24"/>
-      <c r="E130" s="22"/>
-      <c r="F130" s="17" t="s">
+    <row r="130" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="13"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="22"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G130" s="17" t="s">
+      <c r="G130" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="32"/>
-      <c r="B131" s="22"/>
-      <c r="C131" s="26"/>
-      <c r="D131" s="24"/>
-      <c r="E131" s="22"/>
-      <c r="F131" s="17" t="s">
+    <row r="131" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="13"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="19"/>
+      <c r="D131" s="22"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="G131" s="17" t="s">
+      <c r="G131" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="32"/>
-      <c r="B132" s="22"/>
-      <c r="C132" s="26"/>
-      <c r="D132" s="24"/>
-      <c r="E132" s="22"/>
-      <c r="F132" s="17" t="s">
+    <row r="132" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="13"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="19"/>
+      <c r="D132" s="22"/>
+      <c r="E132" s="16"/>
+      <c r="F132" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="G132" s="17" t="s">
+      <c r="G132" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="33"/>
-      <c r="B133" s="23"/>
-      <c r="C133" s="27"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="23"/>
-      <c r="F133" s="17" t="s">
+    <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="14"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="20"/>
+      <c r="D133" s="23"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G133" s="17" t="s">
+      <c r="G133" s="10" t="s">
         <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="A129:A133"/>
-    <mergeCell ref="B129:B133"/>
-    <mergeCell ref="C129:C133"/>
-    <mergeCell ref="D129:D133"/>
-    <mergeCell ref="E129:E133"/>
-    <mergeCell ref="A124:A128"/>
-    <mergeCell ref="B124:B128"/>
-    <mergeCell ref="C124:C128"/>
-    <mergeCell ref="D124:D128"/>
-    <mergeCell ref="E124:E128"/>
-    <mergeCell ref="A119:A123"/>
-    <mergeCell ref="B119:B123"/>
-    <mergeCell ref="C119:C123"/>
-    <mergeCell ref="D119:D123"/>
-    <mergeCell ref="E119:E123"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="C114:C118"/>
-    <mergeCell ref="D114:D118"/>
-    <mergeCell ref="E114:E118"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="B109:B113"/>
-    <mergeCell ref="C109:C113"/>
-    <mergeCell ref="D109:D113"/>
-    <mergeCell ref="E109:E113"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="B104:B108"/>
-    <mergeCell ref="C104:C108"/>
-    <mergeCell ref="D104:D108"/>
-    <mergeCell ref="E104:E108"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="B99:B103"/>
-    <mergeCell ref="C99:C103"/>
-    <mergeCell ref="D99:D103"/>
-    <mergeCell ref="E99:E103"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="D94:D98"/>
-    <mergeCell ref="E94:E98"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="C89:C93"/>
-    <mergeCell ref="D89:D93"/>
-    <mergeCell ref="E89:E93"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="C84:C88"/>
-    <mergeCell ref="D84:D88"/>
-    <mergeCell ref="E84:E88"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="C79:C83"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="E79:E83"/>
-    <mergeCell ref="A74:A78"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="E74:E78"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="C69:C73"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="E69:E73"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="E64:E68"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="B53:B58"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="D53:D58"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="D41:D46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E17:E22"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
@@ -3059,6 +2949,116 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="E59:E63"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="B53:B58"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="D53:D58"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="C69:C73"/>
+    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="E69:E73"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="E64:E68"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="C79:C83"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="E79:E83"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="E89:E93"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="C84:C88"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="C99:C103"/>
+    <mergeCell ref="D99:D103"/>
+    <mergeCell ref="E99:E103"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="D94:D98"/>
+    <mergeCell ref="E94:E98"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="B109:B113"/>
+    <mergeCell ref="C109:C113"/>
+    <mergeCell ref="D109:D113"/>
+    <mergeCell ref="E109:E113"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="C104:C108"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="E104:E108"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="C119:C123"/>
+    <mergeCell ref="D119:D123"/>
+    <mergeCell ref="E119:E123"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="C114:C118"/>
+    <mergeCell ref="D114:D118"/>
+    <mergeCell ref="E114:E118"/>
+    <mergeCell ref="A129:A133"/>
+    <mergeCell ref="B129:B133"/>
+    <mergeCell ref="C129:C133"/>
+    <mergeCell ref="D129:D133"/>
+    <mergeCell ref="E129:E133"/>
+    <mergeCell ref="A124:A128"/>
+    <mergeCell ref="B124:B128"/>
+    <mergeCell ref="C124:C128"/>
+    <mergeCell ref="D124:D128"/>
+    <mergeCell ref="E124:E128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add new test for claim functionality
</commit_message>
<xml_diff>
--- a/docs/Cases.xlsx
+++ b/docs/Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730E3E19-6AC9-44FA-BCCF-771F6976B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69585164-737A-4DD0-A6E1-634FA9A65E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Набор тест кейсов по LogIn и Lo" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,6 @@
     <t>4. Предупреждение по полям с обязательным заполнением</t>
   </si>
   <si>
-    <t>Создание новой заявки с пустыми полями</t>
-  </si>
-  <si>
     <t>Проверить функционал создания заявки на обязательность заполнения полей</t>
   </si>
   <si>
@@ -545,6 +542,9 @@
   </si>
   <si>
     <t>1.4.6</t>
+  </si>
+  <si>
+    <t>Попытка создания новой заявки с пустыми полями</t>
   </si>
 </sst>
 </file>
@@ -737,8 +737,45 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,16 +783,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -764,42 +795,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:B63"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1159,19 +1159,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1182,11 +1182,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="33"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1195,11 +1195,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="33"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
@@ -1208,37 +1208,37 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="33"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="33"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="30" t="s">
+      <c r="A7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1247,11 +1247,11 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1260,11 +1260,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1273,37 +1273,37 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1312,11 +1312,11 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="7" t="s">
         <v>27</v>
       </c>
@@ -1338,37 +1338,37 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1377,64 +1377,64 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" s="30" t="s">
+      <c r="A23" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="32"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1443,11 +1443,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="7" t="s">
         <v>37</v>
       </c>
@@ -1456,55 +1456,55 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="32"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1513,11 +1513,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="7" t="s">
         <v>38</v>
       </c>
@@ -1526,55 +1526,55 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="30" t="s">
+      <c r="A35" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="32"/>
+      <c r="E35" s="18"/>
       <c r="F35" s="7" t="s">
         <v>18</v>
       </c>
@@ -1583,11 +1583,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="24"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="7" t="s">
         <v>42</v>
       </c>
@@ -1596,55 +1596,55 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="B41" s="30" t="s">
+      <c r="A41" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="32"/>
+      <c r="E41" s="18"/>
       <c r="F41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1653,11 +1653,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
       <c r="F42" s="7" t="s">
         <v>42</v>
       </c>
@@ -1666,11 +1666,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="24"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="7" t="s">
         <v>46</v>
       </c>
@@ -1679,46 +1679,46 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="B47" s="30" t="s">
+      <c r="A47" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="32"/>
+      <c r="E47" s="18"/>
       <c r="F47" s="7" t="s">
         <v>18</v>
       </c>
@@ -1727,11 +1727,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
       <c r="F48" s="7" t="s">
         <v>42</v>
       </c>
@@ -1740,11 +1740,11 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="7" t="s">
         <v>51</v>
       </c>
@@ -1753,46 +1753,46 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="24"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="24"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="25"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="30" t="s">
+      <c r="A53" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E53" s="32"/>
+      <c r="E53" s="18"/>
       <c r="F53" s="7" t="s">
         <v>18</v>
       </c>
@@ -1801,11 +1801,11 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
       <c r="F54" s="7" t="s">
         <v>55</v>
       </c>
@@ -1814,55 +1814,55 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="24"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="B59" s="18" t="s">
+      <c r="A59" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B59" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="D59" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="26"/>
       <c r="F59" s="7" t="s">
         <v>18</v>
       </c>
@@ -1871,11 +1871,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
       <c r="F60" s="7" t="s">
         <v>37</v>
       </c>
@@ -1884,11 +1884,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
       <c r="F61" s="7" t="s">
         <v>57</v>
       </c>
@@ -1897,11 +1897,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="24"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
       <c r="F62" s="10" t="s">
         <v>61</v>
       </c>
@@ -1910,11 +1910,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="25"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
       <c r="F63" s="10" t="s">
         <v>63</v>
       </c>
@@ -1923,19 +1923,19 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B64" s="18" t="s">
+      <c r="A64" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D64" s="21" t="s">
+      <c r="D64" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="28"/>
+      <c r="E64" s="26"/>
       <c r="F64" s="7" t="s">
         <v>18</v>
       </c>
@@ -1944,11 +1944,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="24"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="7" t="s">
         <v>37</v>
       </c>
@@ -1957,11 +1957,11 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="24"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="7" t="s">
         <v>57</v>
       </c>
@@ -1970,11 +1970,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="24"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
       <c r="F67" s="10" t="s">
         <v>65</v>
       </c>
@@ -1983,28 +1983,28 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="25"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B69" s="18" t="s">
+      <c r="A69" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D69" s="21" t="s">
+      <c r="D69" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="28"/>
+      <c r="E69" s="26"/>
       <c r="F69" s="7" t="s">
         <v>18</v>
       </c>
@@ -2013,11 +2013,11 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="24"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="26"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
       <c r="F70" s="7" t="s">
         <v>37</v>
       </c>
@@ -2026,11 +2026,11 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="26"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
       <c r="F71" s="7" t="s">
         <v>57</v>
       </c>
@@ -2039,901 +2039,1011 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="24"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="26"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
       <c r="F72" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="25"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
       <c r="F73" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G73" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B74" s="24" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B74" s="18" t="s">
+      <c r="C74" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="18" t="s">
+      <c r="D74" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="15" t="s">
+      <c r="F74" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="24"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
       <c r="F75" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G75" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G75" s="7" t="s">
+    </row>
+    <row r="76" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="15"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="15"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G76" s="10" t="s">
+      <c r="G77" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="24"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="78" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="25"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
     </row>
     <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B79" s="18" t="s">
+      <c r="A79" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C79" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D79" s="21" t="s">
+      <c r="D79" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E79" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="24"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
-      <c r="E80" s="26"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
       <c r="F80" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G80" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G80" s="7" t="s">
+    </row>
+    <row r="81" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="15"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
+      <c r="F81" s="10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="26"/>
-      <c r="F81" s="10" t="s">
+      <c r="G81" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G81" s="10" t="s">
+    </row>
+    <row r="82" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="15"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
+      <c r="F82" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G82" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
     <row r="83" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="25"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
       <c r="F83" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D84" s="21" t="s">
+      <c r="A84" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D84" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="15" t="s">
+      <c r="E84" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G84" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="24"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
       <c r="F85" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G85" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G85" s="7" t="s">
+    </row>
+    <row r="86" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="15"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="24"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="26"/>
-      <c r="F86" s="10" t="s">
+      <c r="G86" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G86" s="10" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="87" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="24"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
+      <c r="A87" s="15"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
       <c r="F87" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="21"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C89" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G87" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="25"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G88" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D89" s="21" t="s">
+      <c r="D89" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="15" t="s">
+      <c r="E89" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="24"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26"/>
-      <c r="E90" s="26"/>
+      <c r="A90" s="15"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
       <c r="F90" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="15"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="15"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G92" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G90" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="24"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="24"/>
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G92" s="10" t="s">
+    </row>
+    <row r="93" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="21"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="25"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="10" t="s">
+      <c r="G93" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G93" s="10" t="s">
+    </row>
+    <row r="94" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="27" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B94" s="15" t="s">
+      <c r="C94" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C94" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D94" s="21" t="s">
+      <c r="D94" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="15" t="s">
+      <c r="E94" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F94" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G94" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="24"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
+      <c r="A95" s="15"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
       <c r="F95" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G95" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G95" s="10" t="s">
+    </row>
+    <row r="96" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="15"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="24"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
-      <c r="F96" s="10" t="s">
+      <c r="G96" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G96" s="10" t="s">
+    </row>
+    <row r="97" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="15"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G97" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="24"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G97" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
     <row r="98" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="25"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
     </row>
     <row r="99" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="15" t="s">
+      <c r="A99" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B99" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C99" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D99" s="21" t="s">
+      <c r="D99" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="15" t="s">
+      <c r="E99" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="24"/>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-      <c r="E100" s="26"/>
+      <c r="A100" s="15"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
       <c r="F100" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G100" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G100" s="10" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="101" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="24"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
-      <c r="D101" s="26"/>
-      <c r="E101" s="26"/>
+      <c r="A101" s="15"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
       <c r="F101" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G101" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="G101" s="10" t="s">
+    </row>
+    <row r="102" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="15"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="24"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="26"/>
-      <c r="E102" s="26"/>
-      <c r="F102" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="G102" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="25"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
       <c r="F103" s="10"/>
       <c r="G103" s="10"/>
     </row>
     <row r="104" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B104" s="15" t="s">
+      <c r="A104" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B104" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C104" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C104" s="18" t="s">
+      <c r="D104" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F104" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D104" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E104" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F104" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="G104" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="15"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="24"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
-      <c r="F105" s="10" t="s">
+      <c r="G105" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G105" s="10" t="s">
+    </row>
+    <row r="106" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="15"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="24"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="10" t="s">
+      <c r="G106" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G106" s="10" t="s">
+    </row>
+    <row r="107" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="15"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="24"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="26"/>
-      <c r="F107" s="10" t="s">
+      <c r="G107" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G107" s="10" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="25"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="22"/>
+      <c r="C108" s="22"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
       <c r="F108" s="10"/>
       <c r="G108" s="10"/>
     </row>
     <row r="109" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B109" s="15" t="s">
+      <c r="A109" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B109" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C109" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D109" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E109" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="15"/>
+      <c r="B110" s="17"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="15"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="17"/>
+      <c r="F111" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="15"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C109" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D109" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E109" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G109" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="24"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="26"/>
-      <c r="E110" s="26"/>
-      <c r="F110" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G110" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="24"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="26"/>
-      <c r="F111" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="G111" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="24"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="26"/>
-      <c r="E112" s="26"/>
-      <c r="F112" s="10" t="s">
+      <c r="G112" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G112" s="10" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="25"/>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="22"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
     </row>
     <row r="114" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="B114" s="15" t="s">
+      <c r="A114" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C114" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C114" s="18" t="s">
+      <c r="D114" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G114" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="15"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="15"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D114" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E114" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G114" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="24"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="26"/>
-      <c r="D115" s="26"/>
-      <c r="E115" s="26"/>
-      <c r="F115" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G115" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="24"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="26"/>
-      <c r="E116" s="26"/>
-      <c r="F116" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="G116" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="24"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="26"/>
-      <c r="E117" s="26"/>
+      <c r="A117" s="15"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
       <c r="F117" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="25"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="27"/>
-      <c r="E118" s="27"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="22"/>
+      <c r="C118" s="22"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
       <c r="F118" s="10"/>
       <c r="G118" s="10"/>
     </row>
     <row r="119" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="B119" s="15" t="s">
+      <c r="A119" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B119" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C119" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C119" s="18" t="s">
+      <c r="D119" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="28"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="34"/>
+      <c r="E120" s="30"/>
+      <c r="F120" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G120" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="28"/>
+      <c r="B121" s="30"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="34"/>
+      <c r="E121" s="30"/>
+      <c r="F121" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D119" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E119" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F119" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G119" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="13"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="19"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G120" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="13"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="19"/>
-      <c r="D121" s="22"/>
-      <c r="E121" s="16"/>
-      <c r="F121" s="10" t="s">
+      <c r="G121" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="28"/>
+      <c r="B122" s="30"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="34"/>
+      <c r="E122" s="30"/>
+      <c r="F122" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G121" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="13"/>
-      <c r="B122" s="16"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="22"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="10" t="s">
+      <c r="G122" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="G122" s="10" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="14"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="20"/>
-      <c r="D123" s="23"/>
-      <c r="E123" s="17"/>
+      <c r="A123" s="29"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="33"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="31"/>
       <c r="F123" s="10"/>
       <c r="G123" s="10"/>
     </row>
     <row r="124" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B124" s="15" t="s">
+      <c r="A124" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B124" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C124" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D124" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="28"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="34"/>
+      <c r="E125" s="30"/>
+      <c r="F125" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G125" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="28"/>
+      <c r="B126" s="30"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="34"/>
+      <c r="E126" s="30"/>
+      <c r="F126" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G126" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="28"/>
+      <c r="B127" s="30"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="30"/>
+      <c r="F127" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C124" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D124" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E124" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F124" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G124" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="13"/>
-      <c r="B125" s="16"/>
-      <c r="C125" s="19"/>
-      <c r="D125" s="22"/>
-      <c r="E125" s="16"/>
-      <c r="F125" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G125" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="13"/>
-      <c r="B126" s="16"/>
-      <c r="C126" s="19"/>
-      <c r="D126" s="22"/>
-      <c r="E126" s="16"/>
-      <c r="F126" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G126" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="13"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="19"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="16"/>
-      <c r="F127" s="10" t="s">
+      <c r="G127" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="G127" s="10" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="14"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="20"/>
-      <c r="D128" s="23"/>
-      <c r="E128" s="17"/>
+      <c r="A128" s="29"/>
+      <c r="B128" s="31"/>
+      <c r="C128" s="33"/>
+      <c r="D128" s="35"/>
+      <c r="E128" s="31"/>
       <c r="F128" s="10"/>
       <c r="G128" s="10"/>
     </row>
     <row r="129" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B129" s="15" t="s">
+      <c r="A129" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B129" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C129" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D129" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="28"/>
+      <c r="B130" s="30"/>
+      <c r="C130" s="32"/>
+      <c r="D130" s="34"/>
+      <c r="E130" s="30"/>
+      <c r="F130" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G130" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="28"/>
+      <c r="B131" s="30"/>
+      <c r="C131" s="32"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="30"/>
+      <c r="F131" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G131" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="28"/>
+      <c r="B132" s="30"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="30"/>
+      <c r="F132" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G132" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C129" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E129" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F129" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G129" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="13"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="22"/>
-      <c r="E130" s="16"/>
-      <c r="F130" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G130" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="13"/>
-      <c r="B131" s="16"/>
-      <c r="C131" s="19"/>
-      <c r="D131" s="22"/>
-      <c r="E131" s="16"/>
-      <c r="F131" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="G131" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="13"/>
-      <c r="B132" s="16"/>
-      <c r="C132" s="19"/>
-      <c r="D132" s="22"/>
-      <c r="E132" s="16"/>
-      <c r="F132" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G132" s="10" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="14"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="20"/>
-      <c r="D133" s="23"/>
-      <c r="E133" s="17"/>
+      <c r="A133" s="29"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="33"/>
+      <c r="D133" s="35"/>
+      <c r="E133" s="31"/>
       <c r="F133" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G133" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="125">
+    <mergeCell ref="A129:A133"/>
+    <mergeCell ref="B129:B133"/>
+    <mergeCell ref="C129:C133"/>
+    <mergeCell ref="D129:D133"/>
+    <mergeCell ref="E129:E133"/>
+    <mergeCell ref="A124:A128"/>
+    <mergeCell ref="B124:B128"/>
+    <mergeCell ref="C124:C128"/>
+    <mergeCell ref="D124:D128"/>
+    <mergeCell ref="E124:E128"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="C119:C123"/>
+    <mergeCell ref="D119:D123"/>
+    <mergeCell ref="E119:E123"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="C114:C118"/>
+    <mergeCell ref="D114:D118"/>
+    <mergeCell ref="E114:E118"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="B109:B113"/>
+    <mergeCell ref="C109:C113"/>
+    <mergeCell ref="D109:D113"/>
+    <mergeCell ref="E109:E113"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="C104:C108"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="E104:E108"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="C99:C103"/>
+    <mergeCell ref="D99:D103"/>
+    <mergeCell ref="E99:E103"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="D94:D98"/>
+    <mergeCell ref="E94:E98"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="E89:E93"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="C84:C88"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="C79:C83"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="E79:E83"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="C69:C73"/>
+    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="E69:E73"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="E64:E68"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="E59:E63"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="B53:B58"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="D53:D58"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E17:E22"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
@@ -2949,116 +3059,6 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="D41:D46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="B53:B58"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="D53:D58"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="C69:C73"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="E69:E73"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="E64:E68"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="C79:C83"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="E79:E83"/>
-    <mergeCell ref="A74:A78"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="E74:E78"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="C89:C93"/>
-    <mergeCell ref="D89:D93"/>
-    <mergeCell ref="E89:E93"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="C84:C88"/>
-    <mergeCell ref="D84:D88"/>
-    <mergeCell ref="E84:E88"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="B99:B103"/>
-    <mergeCell ref="C99:C103"/>
-    <mergeCell ref="D99:D103"/>
-    <mergeCell ref="E99:E103"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="D94:D98"/>
-    <mergeCell ref="E94:E98"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="B109:B113"/>
-    <mergeCell ref="C109:C113"/>
-    <mergeCell ref="D109:D113"/>
-    <mergeCell ref="E109:E113"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="B104:B108"/>
-    <mergeCell ref="C104:C108"/>
-    <mergeCell ref="D104:D108"/>
-    <mergeCell ref="E104:E108"/>
-    <mergeCell ref="A119:A123"/>
-    <mergeCell ref="B119:B123"/>
-    <mergeCell ref="C119:C123"/>
-    <mergeCell ref="D119:D123"/>
-    <mergeCell ref="E119:E123"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="C114:C118"/>
-    <mergeCell ref="D114:D118"/>
-    <mergeCell ref="E114:E118"/>
-    <mergeCell ref="A129:A133"/>
-    <mergeCell ref="B129:B133"/>
-    <mergeCell ref="C129:C133"/>
-    <mergeCell ref="D129:D133"/>
-    <mergeCell ref="E129:E133"/>
-    <mergeCell ref="A124:A128"/>
-    <mergeCell ref="B124:B128"/>
-    <mergeCell ref="C124:C128"/>
-    <mergeCell ref="D124:D128"/>
-    <mergeCell ref="E124:E128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test for deleting news 1.4.3
</commit_message>
<xml_diff>
--- a/docs/Cases.xlsx
+++ b/docs/Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplomNetology\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61AA22-B457-469B-9A41-664C293AEBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E39AD05-1EEE-456C-96CF-46135D83531E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1545" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,8 +737,45 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,16 +783,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -764,42 +795,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1159,19 +1159,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1182,11 +1182,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="33"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1195,11 +1195,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="33"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
@@ -1208,37 +1208,37 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="33"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="33"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1247,11 +1247,11 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1260,11 +1260,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1273,37 +1273,37 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
@@ -1312,11 +1312,11 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1325,11 +1325,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="7" t="s">
         <v>27</v>
       </c>
@@ -1338,37 +1338,37 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1377,64 +1377,64 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="32"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="7" t="s">
         <v>18</v>
       </c>
@@ -1443,11 +1443,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="7" t="s">
         <v>37</v>
       </c>
@@ -1456,55 +1456,55 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="32"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1513,11 +1513,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="7" t="s">
         <v>38</v>
       </c>
@@ -1526,55 +1526,55 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="32"/>
+      <c r="E35" s="18"/>
       <c r="F35" s="7" t="s">
         <v>18</v>
       </c>
@@ -1583,11 +1583,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="24"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="7" t="s">
         <v>42</v>
       </c>
@@ -1596,55 +1596,55 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="32"/>
+      <c r="E41" s="18"/>
       <c r="F41" s="7" t="s">
         <v>18</v>
       </c>
@@ -1653,11 +1653,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
       <c r="F42" s="7" t="s">
         <v>42</v>
       </c>
@@ -1666,11 +1666,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="24"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="7" t="s">
         <v>46</v>
       </c>
@@ -1679,46 +1679,46 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="25"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="32"/>
+      <c r="E47" s="18"/>
       <c r="F47" s="7" t="s">
         <v>18</v>
       </c>
@@ -1727,11 +1727,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
       <c r="F48" s="7" t="s">
         <v>42</v>
       </c>
@@ -1740,11 +1740,11 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="7" t="s">
         <v>51</v>
       </c>
@@ -1753,46 +1753,46 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="24"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="24"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="25"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E53" s="32"/>
+      <c r="E53" s="18"/>
       <c r="F53" s="7" t="s">
         <v>18</v>
       </c>
@@ -1801,11 +1801,11 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
       <c r="F54" s="7" t="s">
         <v>55</v>
       </c>
@@ -1814,55 +1814,55 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="24"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="D59" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="26"/>
       <c r="F59" s="7" t="s">
         <v>18</v>
       </c>
@@ -1871,11 +1871,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
       <c r="F60" s="7" t="s">
         <v>37</v>
       </c>
@@ -1884,11 +1884,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
       <c r="F61" s="7" t="s">
         <v>57</v>
       </c>
@@ -1897,11 +1897,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="24"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
       <c r="F62" s="10" t="s">
         <v>61</v>
       </c>
@@ -1910,11 +1910,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="25"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
       <c r="F63" s="10" t="s">
         <v>63</v>
       </c>
@@ -1923,19 +1923,19 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D64" s="21" t="s">
+      <c r="D64" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="28"/>
+      <c r="E64" s="26"/>
       <c r="F64" s="7" t="s">
         <v>18</v>
       </c>
@@ -1944,11 +1944,11 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="24"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="26"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
       <c r="F65" s="7" t="s">
         <v>37</v>
       </c>
@@ -1957,11 +1957,11 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="24"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="7" t="s">
         <v>57</v>
       </c>
@@ -1970,11 +1970,11 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="24"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
       <c r="F67" s="10" t="s">
         <v>65</v>
       </c>
@@ -1983,28 +1983,28 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="25"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
     </row>
     <row r="69" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D69" s="21" t="s">
+      <c r="D69" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="28"/>
+      <c r="E69" s="26"/>
       <c r="F69" s="7" t="s">
         <v>18</v>
       </c>
@@ -2013,11 +2013,11 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="24"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="26"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
       <c r="F70" s="7" t="s">
         <v>37</v>
       </c>
@@ -2026,11 +2026,11 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="26"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
       <c r="F71" s="7" t="s">
         <v>57</v>
       </c>
@@ -2039,11 +2039,11 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="24"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="26"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
       <c r="F72" s="10" t="s">
         <v>70</v>
       </c>
@@ -2052,11 +2052,11 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="25"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
       <c r="F73" s="10" t="s">
         <v>63</v>
       </c>
@@ -2065,19 +2065,19 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D74" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F74" s="7" t="s">
@@ -2088,11 +2088,11 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="24"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
       <c r="F75" s="7" t="s">
         <v>76</v>
       </c>
@@ -2101,11 +2101,11 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
+      <c r="A76" s="15"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
       <c r="F76" s="10" t="s">
         <v>79</v>
       </c>
@@ -2114,11 +2114,11 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="24"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="26"/>
-      <c r="E77" s="26"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
       <c r="F77" s="10" t="s">
         <v>78</v>
       </c>
@@ -2127,28 +2127,28 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="25"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
     </row>
     <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D79" s="21" t="s">
+      <c r="D79" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E79" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F79" s="7" t="s">
@@ -2159,11 +2159,11 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="24"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="26"/>
-      <c r="E80" s="26"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
       <c r="F80" s="7" t="s">
         <v>84</v>
       </c>
@@ -2172,11 +2172,11 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="26"/>
+      <c r="A81" s="15"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
       <c r="F81" s="10" t="s">
         <v>86</v>
       </c>
@@ -2185,11 +2185,11 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26"/>
-      <c r="E82" s="26"/>
+      <c r="A82" s="15"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="17"/>
       <c r="F82" s="10" t="s">
         <v>89</v>
       </c>
@@ -2198,11 +2198,11 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="25"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
       <c r="F83" s="10" t="s">
         <v>63</v>
       </c>
@@ -2211,19 +2211,19 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C84" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="21" t="s">
+      <c r="D84" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="15" t="s">
+      <c r="E84" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F84" s="7" t="s">
@@ -2234,11 +2234,11 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="24"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17"/>
       <c r="F85" s="7" t="s">
         <v>84</v>
       </c>
@@ -2247,11 +2247,11 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="24"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="26"/>
+      <c r="A86" s="15"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
       <c r="F86" s="10" t="s">
         <v>86</v>
       </c>
@@ -2260,11 +2260,11 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="24"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
+      <c r="A87" s="15"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
       <c r="F87" s="10" t="s">
         <v>91</v>
       </c>
@@ -2273,11 +2273,11 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="25"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
+      <c r="A88" s="21"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
       <c r="F88" s="10" t="s">
         <v>93</v>
       </c>
@@ -2286,19 +2286,19 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C89" s="18" t="s">
+      <c r="C89" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="21" t="s">
+      <c r="D89" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="15" t="s">
+      <c r="E89" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F89" s="7" t="s">
@@ -2309,11 +2309,11 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="24"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26"/>
-      <c r="E90" s="26"/>
+      <c r="A90" s="15"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
       <c r="F90" s="7" t="s">
         <v>98</v>
       </c>
@@ -2322,11 +2322,11 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="24"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
+      <c r="A91" s="15"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
       <c r="F91" s="10" t="s">
         <v>86</v>
       </c>
@@ -2335,11 +2335,11 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="24"/>
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
+      <c r="A92" s="15"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
       <c r="F92" s="10" t="s">
         <v>91</v>
       </c>
@@ -2348,11 +2348,11 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="25"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
+      <c r="A93" s="21"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
       <c r="F93" s="10" t="s">
         <v>100</v>
       </c>
@@ -2361,19 +2361,19 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="12" t="s">
+      <c r="A94" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="D94" s="21" t="s">
+      <c r="D94" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E94" s="15" t="s">
+      <c r="E94" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F94" s="7" t="s">
@@ -2384,11 +2384,11 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="24"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
+      <c r="A95" s="15"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
       <c r="F95" s="10" t="s">
         <v>104</v>
       </c>
@@ -2397,11 +2397,11 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="24"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
+      <c r="A96" s="15"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
       <c r="F96" s="10" t="s">
         <v>106</v>
       </c>
@@ -2410,11 +2410,11 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="24"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
+      <c r="A97" s="15"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
       <c r="F97" s="10" t="s">
         <v>114</v>
       </c>
@@ -2423,28 +2423,28 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="25"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
     </row>
     <row r="99" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="12" t="s">
+      <c r="A99" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C99" s="18" t="s">
+      <c r="C99" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D99" s="21" t="s">
+      <c r="D99" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="15" t="s">
+      <c r="E99" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F99" s="7" t="s">
@@ -2455,11 +2455,11 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="24"/>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-      <c r="E100" s="26"/>
+      <c r="A100" s="15"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
       <c r="F100" s="10" t="s">
         <v>104</v>
       </c>
@@ -2468,11 +2468,11 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="24"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
-      <c r="D101" s="26"/>
-      <c r="E101" s="26"/>
+      <c r="A101" s="15"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
       <c r="F101" s="10" t="s">
         <v>111</v>
       </c>
@@ -2481,11 +2481,11 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="24"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="26"/>
-      <c r="E102" s="26"/>
+      <c r="A102" s="15"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
       <c r="F102" s="10" t="s">
         <v>113</v>
       </c>
@@ -2494,28 +2494,28 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="25"/>
-      <c r="B103" s="27"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
       <c r="F103" s="10"/>
       <c r="G103" s="10"/>
     </row>
     <row r="104" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C104" s="18" t="s">
+      <c r="C104" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D104" s="21" t="s">
+      <c r="D104" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="15" t="s">
+      <c r="E104" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F104" s="7" t="s">
@@ -2526,11 +2526,11 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="24"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
+      <c r="A105" s="15"/>
+      <c r="B105" s="17"/>
+      <c r="C105" s="17"/>
+      <c r="D105" s="17"/>
+      <c r="E105" s="17"/>
       <c r="F105" s="10" t="s">
         <v>121</v>
       </c>
@@ -2539,11 +2539,11 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="24"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
+      <c r="A106" s="15"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
       <c r="F106" s="10" t="s">
         <v>123</v>
       </c>
@@ -2552,11 +2552,11 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="24"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="26"/>
+      <c r="A107" s="15"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
       <c r="F107" s="10" t="s">
         <v>125</v>
       </c>
@@ -2565,28 +2565,28 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="25"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="22"/>
+      <c r="C108" s="22"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
       <c r="F108" s="10"/>
       <c r="G108" s="10"/>
     </row>
     <row r="109" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="12" t="s">
+      <c r="A109" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="C109" s="18" t="s">
+      <c r="C109" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D109" s="21" t="s">
+      <c r="D109" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E109" s="15" t="s">
+      <c r="E109" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F109" s="7" t="s">
@@ -2597,11 +2597,11 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="24"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="26"/>
-      <c r="E110" s="26"/>
+      <c r="A110" s="15"/>
+      <c r="B110" s="17"/>
+      <c r="C110" s="17"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
       <c r="F110" s="10" t="s">
         <v>121</v>
       </c>
@@ -2610,11 +2610,11 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="24"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="26"/>
+      <c r="A111" s="15"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="17"/>
       <c r="F111" s="10" t="s">
         <v>134</v>
       </c>
@@ -2623,11 +2623,11 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="24"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="26"/>
-      <c r="E112" s="26"/>
+      <c r="A112" s="15"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
       <c r="F112" s="10" t="s">
         <v>128</v>
       </c>
@@ -2636,28 +2636,28 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="25"/>
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="22"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
       <c r="F113" s="10"/>
       <c r="G113" s="10"/>
     </row>
     <row r="114" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="12" t="s">
+      <c r="A114" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C114" s="18" t="s">
+      <c r="C114" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="D114" s="21" t="s">
+      <c r="D114" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E114" s="15" t="s">
+      <c r="E114" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F114" s="7" t="s">
@@ -2668,11 +2668,11 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="24"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="26"/>
-      <c r="D115" s="26"/>
-      <c r="E115" s="26"/>
+      <c r="A115" s="15"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
       <c r="F115" s="10" t="s">
         <v>121</v>
       </c>
@@ -2681,11 +2681,11 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="24"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="26"/>
-      <c r="E116" s="26"/>
+      <c r="A116" s="15"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
       <c r="F116" s="10" t="s">
         <v>132</v>
       </c>
@@ -2694,11 +2694,11 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="24"/>
-      <c r="B117" s="26"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="26"/>
-      <c r="E117" s="26"/>
+      <c r="A117" s="15"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
       <c r="F117" s="10" t="s">
         <v>78</v>
       </c>
@@ -2707,28 +2707,28 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="25"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="27"/>
-      <c r="E118" s="27"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="22"/>
+      <c r="C118" s="22"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
       <c r="F118" s="10"/>
       <c r="G118" s="10"/>
     </row>
     <row r="119" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C119" s="18" t="s">
+      <c r="C119" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="D119" s="21" t="s">
+      <c r="D119" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="15" t="s">
+      <c r="E119" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F119" s="7" t="s">
@@ -2739,11 +2739,11 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="13"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="19"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="16"/>
+      <c r="A120" s="28"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="32"/>
+      <c r="D120" s="34"/>
+      <c r="E120" s="30"/>
       <c r="F120" s="10" t="s">
         <v>121</v>
       </c>
@@ -2752,11 +2752,11 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="13"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="19"/>
-      <c r="D121" s="22"/>
-      <c r="E121" s="16"/>
+      <c r="A121" s="28"/>
+      <c r="B121" s="30"/>
+      <c r="C121" s="32"/>
+      <c r="D121" s="34"/>
+      <c r="E121" s="30"/>
       <c r="F121" s="10" t="s">
         <v>138</v>
       </c>
@@ -2765,11 +2765,11 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="13"/>
-      <c r="B122" s="16"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="22"/>
-      <c r="E122" s="16"/>
+      <c r="A122" s="28"/>
+      <c r="B122" s="30"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="34"/>
+      <c r="E122" s="30"/>
       <c r="F122" s="10" t="s">
         <v>139</v>
       </c>
@@ -2778,28 +2778,28 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="14"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="20"/>
-      <c r="D123" s="23"/>
-      <c r="E123" s="17"/>
+      <c r="A123" s="29"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="33"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="31"/>
       <c r="F123" s="10"/>
       <c r="G123" s="10"/>
     </row>
     <row r="124" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="12" t="s">
+      <c r="A124" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="B124" s="15" t="s">
+      <c r="B124" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C124" s="18" t="s">
+      <c r="C124" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="D124" s="21" t="s">
+      <c r="D124" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E124" s="15" t="s">
+      <c r="E124" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F124" s="7" t="s">
@@ -2810,11 +2810,11 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="13"/>
-      <c r="B125" s="16"/>
-      <c r="C125" s="19"/>
-      <c r="D125" s="22"/>
-      <c r="E125" s="16"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="32"/>
+      <c r="D125" s="34"/>
+      <c r="E125" s="30"/>
       <c r="F125" s="10" t="s">
         <v>121</v>
       </c>
@@ -2823,11 +2823,11 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="13"/>
-      <c r="B126" s="16"/>
-      <c r="C126" s="19"/>
-      <c r="D126" s="22"/>
-      <c r="E126" s="16"/>
+      <c r="A126" s="28"/>
+      <c r="B126" s="30"/>
+      <c r="C126" s="32"/>
+      <c r="D126" s="34"/>
+      <c r="E126" s="30"/>
       <c r="F126" s="10" t="s">
         <v>138</v>
       </c>
@@ -2836,11 +2836,11 @@
       </c>
     </row>
     <row r="127" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="13"/>
-      <c r="B127" s="16"/>
-      <c r="C127" s="19"/>
-      <c r="D127" s="22"/>
-      <c r="E127" s="16"/>
+      <c r="A127" s="28"/>
+      <c r="B127" s="30"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="30"/>
       <c r="F127" s="10" t="s">
         <v>143</v>
       </c>
@@ -2849,28 +2849,28 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="14"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="20"/>
-      <c r="D128" s="23"/>
-      <c r="E128" s="17"/>
+      <c r="A128" s="29"/>
+      <c r="B128" s="31"/>
+      <c r="C128" s="33"/>
+      <c r="D128" s="35"/>
+      <c r="E128" s="31"/>
       <c r="F128" s="10"/>
       <c r="G128" s="10"/>
     </row>
     <row r="129" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B129" s="15" t="s">
+      <c r="B129" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="C129" s="18" t="s">
+      <c r="C129" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D129" s="21" t="s">
+      <c r="D129" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E129" s="15" t="s">
+      <c r="E129" s="27" t="s">
         <v>74</v>
       </c>
       <c r="F129" s="7" t="s">
@@ -2881,11 +2881,11 @@
       </c>
     </row>
     <row r="130" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="13"/>
-      <c r="B130" s="16"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="22"/>
-      <c r="E130" s="16"/>
+      <c r="A130" s="28"/>
+      <c r="B130" s="30"/>
+      <c r="C130" s="32"/>
+      <c r="D130" s="34"/>
+      <c r="E130" s="30"/>
       <c r="F130" s="10" t="s">
         <v>121</v>
       </c>
@@ -2894,11 +2894,11 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="13"/>
-      <c r="B131" s="16"/>
-      <c r="C131" s="19"/>
-      <c r="D131" s="22"/>
-      <c r="E131" s="16"/>
+      <c r="A131" s="28"/>
+      <c r="B131" s="30"/>
+      <c r="C131" s="32"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="30"/>
       <c r="F131" s="10" t="s">
         <v>134</v>
       </c>
@@ -2907,11 +2907,11 @@
       </c>
     </row>
     <row r="132" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="13"/>
-      <c r="B132" s="16"/>
-      <c r="C132" s="19"/>
-      <c r="D132" s="22"/>
-      <c r="E132" s="16"/>
+      <c r="A132" s="28"/>
+      <c r="B132" s="30"/>
+      <c r="C132" s="32"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="30"/>
       <c r="F132" s="10" t="s">
         <v>148</v>
       </c>
@@ -2920,11 +2920,11 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="14"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="20"/>
-      <c r="D133" s="23"/>
-      <c r="E133" s="17"/>
+      <c r="A133" s="29"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="33"/>
+      <c r="D133" s="35"/>
+      <c r="E133" s="31"/>
       <c r="F133" s="10" t="s">
         <v>63</v>
       </c>
@@ -2934,6 +2934,116 @@
     </row>
   </sheetData>
   <mergeCells count="125">
+    <mergeCell ref="A129:A133"/>
+    <mergeCell ref="B129:B133"/>
+    <mergeCell ref="C129:C133"/>
+    <mergeCell ref="D129:D133"/>
+    <mergeCell ref="E129:E133"/>
+    <mergeCell ref="A124:A128"/>
+    <mergeCell ref="B124:B128"/>
+    <mergeCell ref="C124:C128"/>
+    <mergeCell ref="D124:D128"/>
+    <mergeCell ref="E124:E128"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="C119:C123"/>
+    <mergeCell ref="D119:D123"/>
+    <mergeCell ref="E119:E123"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="C114:C118"/>
+    <mergeCell ref="D114:D118"/>
+    <mergeCell ref="E114:E118"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="B109:B113"/>
+    <mergeCell ref="C109:C113"/>
+    <mergeCell ref="D109:D113"/>
+    <mergeCell ref="E109:E113"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="C104:C108"/>
+    <mergeCell ref="D104:D108"/>
+    <mergeCell ref="E104:E108"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="C99:C103"/>
+    <mergeCell ref="D99:D103"/>
+    <mergeCell ref="E99:E103"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="D94:D98"/>
+    <mergeCell ref="E94:E98"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="E89:E93"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="C84:C88"/>
+    <mergeCell ref="D84:D88"/>
+    <mergeCell ref="E84:E88"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="C79:C83"/>
+    <mergeCell ref="D79:D83"/>
+    <mergeCell ref="E79:E83"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="D74:D78"/>
+    <mergeCell ref="E74:E78"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="C69:C73"/>
+    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="E69:E73"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="E64:E68"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="E59:E63"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="B53:B58"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="D53:D58"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E17:E22"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
@@ -2949,116 +3059,6 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="D41:D46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="B53:B58"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="D53:D58"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="C69:C73"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="E69:E73"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="E64:E68"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="C79:C83"/>
-    <mergeCell ref="D79:D83"/>
-    <mergeCell ref="E79:E83"/>
-    <mergeCell ref="A74:A78"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="D74:D78"/>
-    <mergeCell ref="E74:E78"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="C89:C93"/>
-    <mergeCell ref="D89:D93"/>
-    <mergeCell ref="E89:E93"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="C84:C88"/>
-    <mergeCell ref="D84:D88"/>
-    <mergeCell ref="E84:E88"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="B99:B103"/>
-    <mergeCell ref="C99:C103"/>
-    <mergeCell ref="D99:D103"/>
-    <mergeCell ref="E99:E103"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="D94:D98"/>
-    <mergeCell ref="E94:E98"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="B109:B113"/>
-    <mergeCell ref="C109:C113"/>
-    <mergeCell ref="D109:D113"/>
-    <mergeCell ref="E109:E113"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="B104:B108"/>
-    <mergeCell ref="C104:C108"/>
-    <mergeCell ref="D104:D108"/>
-    <mergeCell ref="E104:E108"/>
-    <mergeCell ref="A119:A123"/>
-    <mergeCell ref="B119:B123"/>
-    <mergeCell ref="C119:C123"/>
-    <mergeCell ref="D119:D123"/>
-    <mergeCell ref="E119:E123"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="C114:C118"/>
-    <mergeCell ref="D114:D118"/>
-    <mergeCell ref="E114:E118"/>
-    <mergeCell ref="A129:A133"/>
-    <mergeCell ref="B129:B133"/>
-    <mergeCell ref="C129:C133"/>
-    <mergeCell ref="D129:D133"/>
-    <mergeCell ref="E129:E133"/>
-    <mergeCell ref="A124:A128"/>
-    <mergeCell ref="B124:B128"/>
-    <mergeCell ref="C124:C128"/>
-    <mergeCell ref="D124:D128"/>
-    <mergeCell ref="E124:E128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>